<commit_message>
feat(step2): Add enhanced marking scheme extraction notebook with multi-sheet Excel output
- Add new enhanced notebook `step2_generate_marking_scheme_excel_enhanced.ipynb` with comprehensive features
- Implement multi-sheet Excel output with 4 professional sheets (Marking Scheme, Summary, Question Overview, Validation)
- Add advanced Gemini integration with Pydantic validation for structured data extraction
- Implement comprehensive error handling with retry logic and fallback processing
- Add enhanced validation for question completeness and data integrity checks
- Include automatic backup protection for existing Excel files
- Add professional formatting and stakeholder-ready report generation
- Update README.md with Step 2 enhanced features documentation
- Update sample marking scheme Excel file with enhanced output format
- Improve documentation with checkmarks and detailed feature descriptions
</commit_message>
<xml_diff>
--- a/sample/VTC Test Marking Scheme.xlsx
+++ b/sample/VTC Test Marking Scheme.xlsx
@@ -9,6 +9,8 @@
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Marking Scheme" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Summary" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Question Overview" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Validation" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -469,17 +471,20 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>- **Definition (2 marks)**: Correctly stating "**Vocational and Professional Education and Training**".
-- **Focus (4 marks)**: Explaining that it focuses on **practical skills** or **specialized trades**.
-- **Workforce Impact (4 marks)**: Explaining the benefit to the workforce (e.g., **reducing skills gap**, **employment readiness**, supporting the economy).
-**Grading Note**: Apply the 0-10 scale rubric based on the clarity of explanation and use of terminology.
+          <t>**Model Answer:**
+VPET stands for **Vocational and Professional Education and Training**. It is important because it provides students with practical skills and specialized knowledge needed by industries, ensuring Hong Kong has a skilled labor force to support the economy.
+**Marking Breakdown:**
+- Correctly stating "Vocational and Professional Education and Training" (2 marks)
+- Explaining that it focuses on **practical skills** or **specialized trades** (4 marks)
+- Explaining the benefit to the workforce (reducing skills gap, employment readiness) (4 marks)
 ---
 **General Grading Guide:**
-### General Rubric for Partial Marks (0-10 Scale)
-- **9-10 marks**: The answer is complete, accurate, uses correct terminology, and is well-explained.
-- **6-8 marks**: The answer is mostly correct but misses a specific detail (e.g., forgets the full name of a diploma) or the explanation is slightly vague.
-- **3-5 marks**: The student shows basic understanding but misses the core point or only answers half the question.
-- **0-2 marks**: The answer is largely incorrect, irrelevant, or blank.</t>
+### General Grading Guide (0-10 Scale)
+Use the following rubric to determine the score for each question based on the completeness and accuracy of the response:
+- **9-10 marks:** The answer is complete, accurate, uses correct terminology, and is well-explained.
+- **6-8 marks:** The answer is mostly correct but misses a specific detail (e.g., forgets the full name of a diploma) or the explanation is slightly vague.
+- **3-5 marks:** The student shows basic understanding but misses the core point or only answers half the question.
+- **0-2 marks:** The answer is largely incorrect, irrelevant, or blank.</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -499,16 +504,19 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>- **IVE Qualification (5 marks)**: Correctly identifying that **IVE** primarily focuses on **Higher Diploma (HD)** programmes or technical training.
-- **THEi Qualification (5 marks)**: Correctly identifying that **THEi** focuses on vocationally-oriented **Bachelor’s Degree** programmes.
-**Grading Note**: Full marks require identifying both specific qualification types. Partial marks (6-8) if one is vague.
+          <t>**Model Answer:**
+**IVE** primarily focuses on **Higher Diploma (HD)** programmes which are practical and technical in nature. **THEi** focuses on vocationally-oriented **Bachelor’s Degree** programmes that combine practical application with higher-level theory.
+**Marking Breakdown:**
+- Correctly identifying that IVE offers Higher Diplomas/Technical training (5 marks)
+- Correctly identifying that THEi offers Bachelor's Degrees (5 marks)
 ---
 **General Grading Guide:**
-### General Rubric for Partial Marks (0-10 Scale)
-- **9-10 marks**: The answer is complete, accurate, uses correct terminology, and is well-explained.
-- **6-8 marks**: The answer is mostly correct but misses a specific detail (e.g., forgets the full name of a diploma) or the explanation is slightly vague.
-- **3-5 marks**: The student shows basic understanding but misses the core point or only answers half the question.
-- **0-2 marks**: The answer is largely incorrect, irrelevant, or blank.</t>
+### General Grading Guide (0-10 Scale)
+Use the following rubric to determine the score for each question based on the completeness and accuracy of the response:
+- **9-10 marks:** The answer is complete, accurate, uses correct terminology, and is well-explained.
+- **6-8 marks:** The answer is mostly correct but misses a specific detail (e.g., forgets the full name of a diploma) or the explanation is slightly vague.
+- **3-5 marks:** The student shows basic understanding but misses the core point or only answers half the question.
+- **0-2 marks:** The answer is largely incorrect, irrelevant, or blank.</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -528,17 +536,20 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>- **"Think" Component (3 marks)**: Explaining the focus on **theory** or **academic knowledge**.
-- **"Do" Component (3 marks)**: Explaining the focus on **practical skills** or **hands-on** execution.
-- **Synthesis (4 marks)**: Explaining the integration of both (e.g., **solving problems** by combining head and hands).
-**Grading Note**: A score of 9-10 requires a clear explanation of how the two components work together.
+          <t>**Model Answer:**
+This approach cultivates the ability to apply brainpower (theory/thinking) to practical work (doing). It ensures students understand the theory behind their work while also possessing the hands-on technical skills to execute it.
+**Marking Breakdown:**
+- Explaining "Think" (Theory/Academic knowledge) (3 marks)
+- Explaining "Do" (Practical skills/Hands-on) (3 marks)
+- Explaining the synthesis: Being able to solve problems by combining both head and hands (4 marks)
 ---
 **General Grading Guide:**
-### General Rubric for Partial Marks (0-10 Scale)
-- **9-10 marks**: The answer is complete, accurate, uses correct terminology, and is well-explained.
-- **6-8 marks**: The answer is mostly correct but misses a specific detail (e.g., forgets the full name of a diploma) or the explanation is slightly vague.
-- **3-5 marks**: The student shows basic understanding but misses the core point or only answers half the question.
-- **0-2 marks**: The answer is largely incorrect, irrelevant, or blank.</t>
+### General Grading Guide (0-10 Scale)
+Use the following rubric to determine the score for each question based on the completeness and accuracy of the response:
+- **9-10 marks:** The answer is complete, accurate, uses correct terminology, and is well-explained.
+- **6-8 marks:** The answer is mostly correct but misses a specific detail (e.g., forgets the full name of a diploma) or the explanation is slightly vague.
+- **3-5 marks:** The student shows basic understanding but misses the core point or only answers half the question.
+- **0-2 marks:** The answer is largely incorrect, irrelevant, or blank.</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -558,16 +569,19 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>- **Programme Identification (5 marks)**: Correctly naming the "**Diploma of Foundation Studies**" (DFS) or "**Diploma of Vocational Education**" (DVE).
-- **Progression Pathway (5 marks)**: Explaining that successful completion allows/guarantees entry to **Higher Diploma (HD)** programmes.
-**Grading Note**: If the student misses the specific name but describes the pathway, award 3-5 marks.
+          <t>**Model Answer:**
+The student can enroll in the **Diploma of Foundation Studies (DFS)** (or Diploma of Vocational Education). Upon successful completion of this diploma, they are eligible to progress to VTC **Higher Diploma (HD)** programmes.
+**Marking Breakdown:**
+- Correctly naming the "Diploma of Foundation Studies" (DFS) or "Diploma of Vocational Education" (DVE) (5 marks)
+- Explanation of the progression (Completion of DFS guarantees/allows entry to Higher Diploma) (5 marks)
 ---
 **General Grading Guide:**
-### General Rubric for Partial Marks (0-10 Scale)
-- **9-10 marks**: The answer is complete, accurate, uses correct terminology, and is well-explained.
-- **6-8 marks**: The answer is mostly correct but misses a specific detail (e.g., forgets the full name of a diploma) or the explanation is slightly vague.
-- **3-5 marks**: The student shows basic understanding but misses the core point or only answers half the question.
-- **0-2 marks**: The answer is largely incorrect, irrelevant, or blank.</t>
+### General Grading Guide (0-10 Scale)
+Use the following rubric to determine the score for each question based on the completeness and accuracy of the response:
+- **9-10 marks:** The answer is complete, accurate, uses correct terminology, and is well-explained.
+- **6-8 marks:** The answer is mostly correct but misses a specific detail (e.g., forgets the full name of a diploma) or the explanation is slightly vague.
+- **3-5 marks:** The student shows basic understanding but misses the core point or only answers half the question.
+- **0-2 marks:** The answer is largely incorrect, irrelevant, or blank.</t>
         </is>
       </c>
       <c r="D5" t="n">
@@ -587,17 +601,20 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>- **General Rationale (4 marks)**: Explaining that collaboration ensures **curriculum relevance** or meets **market trends/industry needs**.
-- **Benefit Example 1 (3 marks)**: e.g., **Internships** or Work-integrated learning.
-- **Benefit Example 2 (3 marks)**: e.g., **Job placement support** or access to **industry-standard equipment**.
-**Grading Note**: To achieve 9-10 marks, the student must provide two distinct and valid benefits.
+          <t>**Model Answer:**
+Collaboration ensures the curriculum is up-to-date with market trends. Benefits include: (1) Internship/Work-integrated learning opportunities, (2) Job placement support, (3) Access to industry-standard equipment/facilities.
+**Marking Breakdown:**
+- General explanation (Curriculum relevance/Industry needs) (4 marks)
+- First specific benefit (e.g., Internships) (3 marks)
+- Second specific benefit (e.g., Job prospects or Equipment) (3 marks)
 ---
 **General Grading Guide:**
-### General Rubric for Partial Marks (0-10 Scale)
-- **9-10 marks**: The answer is complete, accurate, uses correct terminology, and is well-explained.
-- **6-8 marks**: The answer is mostly correct but misses a specific detail (e.g., forgets the full name of a diploma) or the explanation is slightly vague.
-- **3-5 marks**: The student shows basic understanding but misses the core point or only answers half the question.
-- **0-2 marks**: The answer is largely incorrect, irrelevant, or blank.</t>
+### General Grading Guide (0-10 Scale)
+Use the following rubric to determine the score for each question based on the completeness and accuracy of the response:
+- **9-10 marks:** The answer is complete, accurate, uses correct terminology, and is well-explained.
+- **6-8 marks:** The answer is mostly correct but misses a specific detail (e.g., forgets the full name of a diploma) or the explanation is slightly vague.
+- **3-5 marks:** The student shows basic understanding but misses the core point or only answers half the question.
+- **0-2 marks:** The answer is largely incorrect, irrelevant, or blank.</t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -615,7 +632,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -626,30 +643,302 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>Metric</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
           <t>Total Questions</t>
         </is>
       </c>
+      <c r="B2" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Total Marks</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Average Marks per Question</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>10.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Min Marks per Question</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Max Marks per Question</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Generated On</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>2026-01-04 23:34:09</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Input File</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>VTC Test Marking Scheme.docx</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Output File</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>VTC Test Marking Scheme.xlsx</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>question_number</t>
+        </is>
+      </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Total Marks</t>
+          <t>question_text</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Output File</t>
+          <t>marks</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>5</v>
-      </c>
-      <c r="B2" t="n">
-        <v>50</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>../sample/VTC Test Marking Scheme.xlsx</t>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Q1</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>The VTC is the largest provider of VPET in Hong Kong. Briefly explain what VPET stands for and why it is important for Hong Kong’s workforce development.</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Q2</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Compare IVE (Hong Kong Institute of Vocational Education) and THEi (Technological and Higher Education Institute of Hong Kong). What is the main difference between the types of qualifications/programmes offered by these two institutions?</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Q3</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>VTC emphasizes the "Think and Do" approach. Explain what this phrase means in the context of a student's learning experience.</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Q4</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>If a Secondary 6 student does not achieve the minimum entrance requirements for a Bachelor's Degree or a Higher Diploma, what is the VTC study pathway available to them to eventually reach a Higher Diploma level? (Name the specific foundation programme).</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Q5</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Why does the VTC collaborate closely with industry partners (companies and trade associations)? Give two examples of how this benefits students.</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Check</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>All questions have marking schemes</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>✅ PASS</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>All questions have valid marks</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>✅ PASS</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Question numbers are unique</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>✅ PASS</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Total marks calculated</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>✅ PASS (50 marks)</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>General grading guide processed</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>✅ PROCESSED</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Enhance email scoring notebook and dependencies
- Updated the `step7_email_score.ipynb` notebook with improved markdown formatting and added features for email sending.
- Removed the deprecated `step7_email_score_enhanced.ipynb` notebook.
- Added `seaborn` to development requirements for enhanced data visualization.
- Updated `requirements.txt` to include `PyPDF4` and `seaborn` for improved PDF handling and visualization capabilities.
- Updated the binary `VTC Test Marking Scheme.xlsx` file to reflect recent changes.
</commit_message>
<xml_diff>
--- a/sample/VTC Test Marking Scheme.xlsx
+++ b/sample/VTC Test Marking Scheme.xlsx
@@ -466,7 +466,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>The VTC is the largest provider of VPET in Hong Kong. Briefly explain what VPET stands for and why it is important for Hong Kong’s workforce development.</t>
+          <t>The Role of VTC: The VTC is the largest provider of VPET in Hong Kong. Briefly explain what VPET stands for and why it is important for Hong Kong’s workforce development.</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -479,7 +479,7 @@
 - Explaining the benefit to the workforce (reducing skills gap, employment readiness) (4 marks)
 ---
 **General Grading Guide:**
-### General Grading Guide (0-10 Scale)
+**General Grading Guide (0-10 Scale)**
 Use the following rubric to determine the score for each question based on the completeness and accuracy of the response:
 - **9-10 marks:** The answer is complete, accurate, uses correct terminology, and is well-explained.
 - **6-8 marks:** The answer is mostly correct but misses a specific detail (e.g., forgets the full name of a diploma) or the explanation is slightly vague.
@@ -499,7 +499,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Compare IVE (Hong Kong Institute of Vocational Education) and THEi (Technological and Higher Education Institute of Hong Kong). What is the main difference between the types of qualifications/programmes offered by these two institutions?</t>
+          <t>Member Institutions: Compare IVE (Hong Kong Institute of Vocational Education) and THEi (Technological and Higher Education Institute of Hong Kong). What is the main difference between the types of qualifications/programmes offered by these two institutions?</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -511,7 +511,7 @@
 - Correctly identifying that THEi offers Bachelor's Degrees (5 marks)
 ---
 **General Grading Guide:**
-### General Grading Guide (0-10 Scale)
+**General Grading Guide (0-10 Scale)**
 Use the following rubric to determine the score for each question based on the completeness and accuracy of the response:
 - **9-10 marks:** The answer is complete, accurate, uses correct terminology, and is well-explained.
 - **6-8 marks:** The answer is mostly correct but misses a specific detail (e.g., forgets the full name of a diploma) or the explanation is slightly vague.
@@ -531,7 +531,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>VTC emphasizes the "Think and Do" approach. Explain what this phrase means in the context of a student's learning experience.</t>
+          <t>Educational Philosophy: VTC emphasizes the "Think and Do" approach. Explain what this phrase means in the context of a student's learning experience.</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -544,7 +544,7 @@
 - Explaining the synthesis: Being able to solve problems by combining both head and hands (4 marks)
 ---
 **General Grading Guide:**
-### General Grading Guide (0-10 Scale)
+**General Grading Guide (0-10 Scale)**
 Use the following rubric to determine the score for each question based on the completeness and accuracy of the response:
 - **9-10 marks:** The answer is complete, accurate, uses correct terminology, and is well-explained.
 - **6-8 marks:** The answer is mostly correct but misses a specific detail (e.g., forgets the full name of a diploma) or the explanation is slightly vague.
@@ -564,7 +564,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>If a Secondary 6 student does not achieve the minimum entrance requirements for a Bachelor's Degree or a Higher Diploma, what is the VTC study pathway available to them to eventually reach a Higher Diploma level? (Name the specific foundation programme).</t>
+          <t>Study Pathways: If a Secondary 6 student does not achieve the minimum entrance requirements for a Bachelor's Degree or a Higher Diploma, what is the VTC study pathway available to them to eventually reach a Higher Diploma level? (Name the specific foundation programme).</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -576,7 +576,7 @@
 - Explanation of the progression (Completion of DFS guarantees/allows entry to Higher Diploma) (5 marks)
 ---
 **General Grading Guide:**
-### General Grading Guide (0-10 Scale)
+**General Grading Guide (0-10 Scale)**
 Use the following rubric to determine the score for each question based on the completeness and accuracy of the response:
 - **9-10 marks:** The answer is complete, accurate, uses correct terminology, and is well-explained.
 - **6-8 marks:** The answer is mostly correct but misses a specific detail (e.g., forgets the full name of a diploma) or the explanation is slightly vague.
@@ -596,7 +596,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Why does the VTC collaborate closely with industry partners (companies and trade associations)? Give two examples of how this benefits students.</t>
+          <t>Industry Partnership: Why does the VTC collaborate closely with industry partners (companies and trade associations)? Give two examples of how this benefits students.</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -609,7 +609,7 @@
 - Second specific benefit (e.g., Job prospects or Equipment) (3 marks)
 ---
 **General Grading Guide:**
-### General Grading Guide (0-10 Scale)
+**General Grading Guide (0-10 Scale)**
 Use the following rubric to determine the score for each question based on the completeness and accuracy of the response:
 - **9-10 marks:** The answer is complete, accurate, uses correct terminology, and is well-explained.
 - **6-8 marks:** The answer is mostly correct but misses a specific detail (e.g., forgets the full name of a diploma) or the explanation is slightly vague.
@@ -712,7 +712,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2026-01-04 23:34:09</t>
+          <t>2026-01-05 01:23:05</t>
         </is>
       </c>
     </row>
@@ -784,7 +784,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>The VTC is the largest provider of VPET in Hong Kong. Briefly explain what VPET stands for and why it is important for Hong Kong’s workforce development.</t>
+          <t>The Role of VTC: The VTC is the largest provider of VPET in Hong Kong. Briefly explain what VPET stands for and why it is important for Hong Kong’s workforce development.</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -799,7 +799,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Compare IVE (Hong Kong Institute of Vocational Education) and THEi (Technological and Higher Education Institute of Hong Kong). What is the main difference between the types of qualifications/programmes offered by these two institutions?</t>
+          <t>Member Institutions: Compare IVE (Hong Kong Institute of Vocational Education) and THEi (Technological and Higher Education Institute of Hong Kong). What is the main difference between the types of qualifications/programmes offered by these two institutions?</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -814,7 +814,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>VTC emphasizes the "Think and Do" approach. Explain what this phrase means in the context of a student's learning experience.</t>
+          <t>Educational Philosophy: VTC emphasizes the "Think and Do" approach. Explain what this phrase means in the context of a student's learning experience.</t>
         </is>
       </c>
       <c r="C4" t="n">
@@ -829,7 +829,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>If a Secondary 6 student does not achieve the minimum entrance requirements for a Bachelor's Degree or a Higher Diploma, what is the VTC study pathway available to them to eventually reach a Higher Diploma level? (Name the specific foundation programme).</t>
+          <t>Study Pathways: If a Secondary 6 student does not achieve the minimum entrance requirements for a Bachelor's Degree or a Higher Diploma, what is the VTC study pathway available to them to eventually reach a Higher Diploma level? (Name the specific foundation programme).</t>
         </is>
       </c>
       <c r="C5" t="n">
@@ -844,7 +844,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Why does the VTC collaborate closely with industry partners (companies and trade associations)? Give two examples of how this benefits students.</t>
+          <t>Industry Partnership: Why does the VTC collaborate closely with industry partners (companies and trade associations)? Give two examples of how this benefits students.</t>
         </is>
       </c>
       <c r="C6" t="n">

</xml_diff>

<commit_message>
Add Fonts for LibreOffice PDF conversion. Fix backup zip. Cleanup cells.
</commit_message>
<xml_diff>
--- a/sample/VTC Test Marking Scheme.xlsx
+++ b/sample/VTC Test Marking Scheme.xlsx
@@ -475,7 +475,7 @@
 VPET stands for **Vocational and Professional Education and Training**. It is important because it provides students with practical skills and specialized knowledge needed by industries, ensuring Hong Kong has a skilled labor force to support the economy.
 **Marking Breakdown:**
 - Correctly stating "Vocational and Professional Education and Training" (2 marks)
-- Explaining that it focuses on **practical skills** or **specialized trades** (4 marks)
+- Explaining that it focuses on _practical skills_ or _specialized trades_ (4 marks)
 - Explaining the benefit to the workforce (reducing skills gap, employment readiness) (4 marks)
 ---
 **General Grading Guide:**
@@ -712,7 +712,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2026-01-05 01:23:05</t>
+          <t>2026-01-05 06:30:51</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
migrate step2 to ADK.
</commit_message>
<xml_diff>
--- a/sample/VTC Test Marking Scheme.xlsx
+++ b/sample/VTC Test Marking Scheme.xlsx
@@ -466,25 +466,25 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>The Role of VTC: The VTC is the largest provider of VPET in Hong Kong. Briefly explain what VPET stands for and why it is important for Hong Kong’s workforce development.</t>
+          <t>The Role of VTC. The VTC is the largest provider of VPET in Hong Kong. Briefly explain what VPET stands for and why it is important for Hong Kong’s workforce development.</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>**Model Answer:**
-VPET stands for **Vocational and Professional Education and Training**. It is important because it provides students with practical skills and specialized knowledge needed by industries, ensuring Hong Kong has a skilled labor force to support the economy.
-**Marking Breakdown:**
-- Correctly stating "Vocational and Professional Education and Training" (2 marks)
-- Explaining that it focuses on _practical skills_ or _specialized trades_ (4 marks)
-- Explaining the benefit to the workforce (reducing skills gap, employment readiness) (4 marks)
+          <t>- **VPET Definition**: Correctly stating **Vocational and Professional Education and Training** (2 marks)
+- **Focus**: Explaining that it focuses on **practical skills** or **specialized trades** (4 marks)
+- **Workforce Benefit**: Explaining the benefit to the workforce, such as reducing skills gap or employment readiness (4 marks)
+**General Rubric Application:**
+- **9-10 marks**: Complete, accurate, uses correct terminology, and well-explained.
+- **6-8 marks**: Mostly correct but misses a specific detail or explanation is slightly vague.
+- **3-5 marks**: Basic understanding but misses core point or only answers half the question.
+- **0-2 marks**: Incorrect, irrelevant, or blank.
 ---
 **General Grading Guide:**
-**General Grading Guide (0-10 Scale)**
-Use the following rubric to determine the score for each question based on the completeness and accuracy of the response:
-- **9-10 marks:** The answer is complete, accurate, uses correct terminology, and is well-explained.
-- **6-8 marks:** The answer is mostly correct but misses a specific detail (e.g., forgets the full name of a diploma) or the explanation is slightly vague.
-- **3-5 marks:** The student shows basic understanding but misses the core point or only answers half the question.
-- **0-2 marks:** The answer is largely incorrect, irrelevant, or blank.</t>
+- **9-10 marks**: The answer is complete, accurate, uses correct terminology, and is well-explained.
+- **6-8 marks**: The answer is mostly correct but misses a specific detail (e.g., forgets the full name of a diploma) or the explanation is slightly vague.
+- **3-5 marks**: The student shows basic understanding but misses the core point or only answers half the question.
+- **0-2 marks**: The answer is largely incorrect, irrelevant, or blank.</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -499,24 +499,24 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Member Institutions: Compare IVE (Hong Kong Institute of Vocational Education) and THEi (Technological and Higher Education Institute of Hong Kong). What is the main difference between the types of qualifications/programmes offered by these two institutions?</t>
+          <t>Member Institutions. Compare IVE (Hong Kong Institute of Vocational Education) and THEi (Technological and Higher Education Institute of Hong Kong). What is the main difference between the types of qualifications/programmes offered by these two institutions?</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>**Model Answer:**
-**IVE** primarily focuses on **Higher Diploma (HD)** programmes which are practical and technical in nature. **THEi** focuses on vocationally-oriented **Bachelor’s Degree** programmes that combine practical application with higher-level theory.
-**Marking Breakdown:**
-- Correctly identifying that IVE offers Higher Diplomas/Technical training (5 marks)
-- Correctly identifying that THEi offers Bachelor's Degrees (5 marks)
+          <t>- **IVE Identification**: Correctly identifying that IVE primarily focuses on **Higher Diploma (HD)** programmes which are practical and technical (5 marks)
+- **THEi Identification**: Correctly identifying that THEi focuses on vocationally-oriented **Bachelor’s Degree** programmes (5 marks)
+**General Rubric Application:**
+- **9-10 marks**: Complete, accurate, uses correct terminology, and well-explained.
+- **6-8 marks**: Mostly correct but misses a specific detail or explanation is slightly vague.
+- **3-5 marks**: Basic understanding but misses core point or only answers half the question.
+- **0-2 marks**: Incorrect, irrelevant, or blank.
 ---
 **General Grading Guide:**
-**General Grading Guide (0-10 Scale)**
-Use the following rubric to determine the score for each question based on the completeness and accuracy of the response:
-- **9-10 marks:** The answer is complete, accurate, uses correct terminology, and is well-explained.
-- **6-8 marks:** The answer is mostly correct but misses a specific detail (e.g., forgets the full name of a diploma) or the explanation is slightly vague.
-- **3-5 marks:** The student shows basic understanding but misses the core point or only answers half the question.
-- **0-2 marks:** The answer is largely incorrect, irrelevant, or blank.</t>
+- **9-10 marks**: The answer is complete, accurate, uses correct terminology, and is well-explained.
+- **6-8 marks**: The answer is mostly correct but misses a specific detail (e.g., forgets the full name of a diploma) or the explanation is slightly vague.
+- **3-5 marks**: The student shows basic understanding but misses the core point or only answers half the question.
+- **0-2 marks**: The answer is largely incorrect, irrelevant, or blank.</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -531,25 +531,25 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Educational Philosophy: VTC emphasizes the "Think and Do" approach. Explain what this phrase means in the context of a student's learning experience.</t>
+          <t>Educational Philosophy. VTC emphasizes the "Think and Do" approach. Explain what this phrase means in the context of a student's learning experience.</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>**Model Answer:**
-This approach cultivates the ability to apply brainpower (theory/thinking) to practical work (doing). It ensures students understand the theory behind their work while also possessing the hands-on technical skills to execute it.
-**Marking Breakdown:**
-- Explaining "Think" (Theory/Academic knowledge) (3 marks)
-- Explaining "Do" (Practical skills/Hands-on) (3 marks)
-- Explaining the synthesis: Being able to solve problems by combining both head and hands (4 marks)
+          <t>- **"Think" Component**: Explaining the application of brainpower, theory, or academic knowledge (3 marks)
+- **"Do" Component**: Explaining the application of practical work, hands-on technical skills, or execution (3 marks)
+- **Synthesis**: Explaining the ability to solve problems by combining both head and hands (4 marks)
+**General Rubric Application:**
+- **9-10 marks**: Complete, accurate, uses correct terminology, and well-explained.
+- **6-8 marks**: Mostly correct but misses a specific detail or explanation is slightly vague.
+- **3-5 marks**: Basic understanding but misses core point or only answers half the question.
+- **0-2 marks**: Incorrect, irrelevant, or blank.
 ---
 **General Grading Guide:**
-**General Grading Guide (0-10 Scale)**
-Use the following rubric to determine the score for each question based on the completeness and accuracy of the response:
-- **9-10 marks:** The answer is complete, accurate, uses correct terminology, and is well-explained.
-- **6-8 marks:** The answer is mostly correct but misses a specific detail (e.g., forgets the full name of a diploma) or the explanation is slightly vague.
-- **3-5 marks:** The student shows basic understanding but misses the core point or only answers half the question.
-- **0-2 marks:** The answer is largely incorrect, irrelevant, or blank.</t>
+- **9-10 marks**: The answer is complete, accurate, uses correct terminology, and is well-explained.
+- **6-8 marks**: The answer is mostly correct but misses a specific detail (e.g., forgets the full name of a diploma) or the explanation is slightly vague.
+- **3-5 marks**: The student shows basic understanding but misses the core point or only answers half the question.
+- **0-2 marks**: The answer is largely incorrect, irrelevant, or blank.</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -564,24 +564,24 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Study Pathways: If a Secondary 6 student does not achieve the minimum entrance requirements for a Bachelor's Degree or a Higher Diploma, what is the VTC study pathway available to them to eventually reach a Higher Diploma level? (Name the specific foundation programme).</t>
+          <t>Study Pathways. If a Secondary 6 student does not achieve the minimum entrance requirements for a Bachelor's Degree or a Higher Diploma, what is the VTC study pathway available to them to eventually reach a Higher Diploma level? (Name the specific foundation programme).</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>**Model Answer:**
-The student can enroll in the **Diploma of Foundation Studies (DFS)** (or Diploma of Vocational Education). Upon successful completion of this diploma, they are eligible to progress to VTC **Higher Diploma (HD)** programmes.
-**Marking Breakdown:**
-- Correctly naming the "Diploma of Foundation Studies" (DFS) or "Diploma of Vocational Education" (DVE) (5 marks)
-- Explanation of the progression (Completion of DFS guarantees/allows entry to Higher Diploma) (5 marks)
+          <t>- **Programme Name**: Correctly naming the **Diploma of Foundation Studies (DFS)** or **Diploma of Vocational Education (DVE)** (5 marks)
+- **Progression Path**: Explaining that successful completion allows progression to **Higher Diploma (HD)** programmes (5 marks)
+**General Rubric Application:**
+- **9-10 marks**: Complete, accurate, uses correct terminology, and well-explained.
+- **6-8 marks**: Mostly correct but misses a specific detail or explanation is slightly vague.
+- **3-5 marks**: Basic understanding but misses core point or only answers half the question.
+- **0-2 marks**: Incorrect, irrelevant, or blank.
 ---
 **General Grading Guide:**
-**General Grading Guide (0-10 Scale)**
-Use the following rubric to determine the score for each question based on the completeness and accuracy of the response:
-- **9-10 marks:** The answer is complete, accurate, uses correct terminology, and is well-explained.
-- **6-8 marks:** The answer is mostly correct but misses a specific detail (e.g., forgets the full name of a diploma) or the explanation is slightly vague.
-- **3-5 marks:** The student shows basic understanding but misses the core point or only answers half the question.
-- **0-2 marks:** The answer is largely incorrect, irrelevant, or blank.</t>
+- **9-10 marks**: The answer is complete, accurate, uses correct terminology, and is well-explained.
+- **6-8 marks**: The answer is mostly correct but misses a specific detail (e.g., forgets the full name of a diploma) or the explanation is slightly vague.
+- **3-5 marks**: The student shows basic understanding but misses the core point or only answers half the question.
+- **0-2 marks**: The answer is largely incorrect, irrelevant, or blank.</t>
         </is>
       </c>
       <c r="D5" t="n">
@@ -596,25 +596,25 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Industry Partnership: Why does the VTC collaborate closely with industry partners (companies and trade associations)? Give two examples of how this benefits students.</t>
+          <t>Industry Partnership. Why does the VTC collaborate closely with industry partners (companies and trade associations)? Give two examples of how this benefits students.</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>**Model Answer:**
-Collaboration ensures the curriculum is up-to-date with market trends. Benefits include: (1) Internship/Work-integrated learning opportunities, (2) Job placement support, (3) Access to industry-standard equipment/facilities.
-**Marking Breakdown:**
-- General explanation (Curriculum relevance/Industry needs) (4 marks)
-- First specific benefit (e.g., Internships) (3 marks)
-- Second specific benefit (e.g., Job prospects or Equipment) (3 marks)
+          <t>- **General Rationale**: Ensuring curriculum is up-to-date with market trends and industry needs (4 marks)
+- **Benefit Example 1**: Specific benefit such as **internships** or work-integrated learning (3 marks)
+- **Benefit Example 2**: Specific benefit such as **job placement support** or access to industry-standard equipment (3 marks)
+**General Rubric Application:**
+- **9-10 marks**: Complete, accurate, uses correct terminology, and well-explained.
+- **6-8 marks**: Mostly correct but misses a specific detail or explanation is slightly vague.
+- **3-5 marks**: Basic understanding but misses core point or only answers half the question.
+- **0-2 marks**: Incorrect, irrelevant, or blank.
 ---
 **General Grading Guide:**
-**General Grading Guide (0-10 Scale)**
-Use the following rubric to determine the score for each question based on the completeness and accuracy of the response:
-- **9-10 marks:** The answer is complete, accurate, uses correct terminology, and is well-explained.
-- **6-8 marks:** The answer is mostly correct but misses a specific detail (e.g., forgets the full name of a diploma) or the explanation is slightly vague.
-- **3-5 marks:** The student shows basic understanding but misses the core point or only answers half the question.
-- **0-2 marks:** The answer is largely incorrect, irrelevant, or blank.</t>
+- **9-10 marks**: The answer is complete, accurate, uses correct terminology, and is well-explained.
+- **6-8 marks**: The answer is mostly correct but misses a specific detail (e.g., forgets the full name of a diploma) or the explanation is slightly vague.
+- **3-5 marks**: The student shows basic understanding but misses the core point or only answers half the question.
+- **0-2 marks**: The answer is largely incorrect, irrelevant, or blank.</t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -712,7 +712,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2026-01-05 06:30:51</t>
+          <t>2026-01-06 06:20:04</t>
         </is>
       </c>
     </row>
@@ -784,7 +784,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>The Role of VTC: The VTC is the largest provider of VPET in Hong Kong. Briefly explain what VPET stands for and why it is important for Hong Kong’s workforce development.</t>
+          <t>The Role of VTC. The VTC is the largest provider of VPET in Hong Kong. Briefly explain what VPET stands for and why it is important for Hong Kong’s workforce development.</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -799,7 +799,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Member Institutions: Compare IVE (Hong Kong Institute of Vocational Education) and THEi (Technological and Higher Education Institute of Hong Kong). What is the main difference between the types of qualifications/programmes offered by these two institutions?</t>
+          <t>Member Institutions. Compare IVE (Hong Kong Institute of Vocational Education) and THEi (Technological and Higher Education Institute of Hong Kong). What is the main difference between the types of qualifications/programmes offered by these two institutions?</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -814,7 +814,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Educational Philosophy: VTC emphasizes the "Think and Do" approach. Explain what this phrase means in the context of a student's learning experience.</t>
+          <t>Educational Philosophy. VTC emphasizes the "Think and Do" approach. Explain what this phrase means in the context of a student's learning experience.</t>
         </is>
       </c>
       <c r="C4" t="n">
@@ -829,7 +829,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Study Pathways: If a Secondary 6 student does not achieve the minimum entrance requirements for a Bachelor's Degree or a Higher Diploma, what is the VTC study pathway available to them to eventually reach a Higher Diploma level? (Name the specific foundation programme).</t>
+          <t>Study Pathways. If a Secondary 6 student does not achieve the minimum entrance requirements for a Bachelor's Degree or a Higher Diploma, what is the VTC study pathway available to them to eventually reach a Higher Diploma level? (Name the specific foundation programme).</t>
         </is>
       </c>
       <c r="C5" t="n">
@@ -844,7 +844,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Industry Partnership: Why does the VTC collaborate closely with industry partners (companies and trade associations)? Give two examples of how this benefits students.</t>
+          <t>Industry Partnership. Why does the VTC collaborate closely with industry partners (companies and trade associations)? Give two examples of how this benefits students.</t>
         </is>
       </c>
       <c r="C6" t="n">

</xml_diff>

<commit_message>
Refactor comon agent code. Change default show image column.
</commit_message>
<xml_diff>
--- a/sample/VTC Test Marking Scheme.xlsx
+++ b/sample/VTC Test Marking Scheme.xlsx
@@ -466,19 +466,19 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>The Role of VTC. The VTC is the largest provider of VPET in Hong Kong. Briefly explain what VPET stands for and why it is important for Hong Kong’s workforce development.</t>
+          <t>The VTC is the largest provider of VPET in Hong Kong. Briefly explain what VPET stands for and why it is important for Hong Kong’s workforce development.</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>- **VPET Definition**: Correctly stating **Vocational and Professional Education and Training** (2 marks)
-- **Focus**: Explaining that it focuses on **practical skills** or **specialized trades** (4 marks)
-- **Workforce Benefit**: Explaining the benefit to the workforce, such as reducing skills gap or employment readiness (4 marks)
-**General Rubric Application:**
-- **9-10 marks**: Complete, accurate, uses correct terminology, and well-explained.
-- **6-8 marks**: Mostly correct but misses a specific detail or explanation is slightly vague.
-- **3-5 marks**: Basic understanding but misses core point or only answers half the question.
-- **0-2 marks**: Incorrect, irrelevant, or blank.
+          <t>- **Vocational and Professional Education and Training** (2 marks)
+- Focus on **practical skills** or **specialized trades** (4 marks)
+- Benefit to workforce: reducing skills gap, employment readiness (4 marks)
+**General Grading Principles:**
+- **9-10 marks**: Complete, accurate, correct terminology.
+- **6-8 marks**: Mostly correct, misses detail.
+- **3-5 marks**: Basic understanding only.
+- **0-2 marks**: Incorrect or irrelevant.
 ---
 **General Grading Guide:**
 - **9-10 marks**: The answer is complete, accurate, uses correct terminology, and is well-explained.
@@ -499,18 +499,18 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Member Institutions. Compare IVE (Hong Kong Institute of Vocational Education) and THEi (Technological and Higher Education Institute of Hong Kong). What is the main difference between the types of qualifications/programmes offered by these two institutions?</t>
+          <t>Compare IVE (Hong Kong Institute of Vocational Education) and THEi (Technological and Higher Education Institute of Hong Kong). What is the main difference between the types of qualifications/programmes offered by these two institutions?</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>- **IVE Identification**: Correctly identifying that IVE primarily focuses on **Higher Diploma (HD)** programmes which are practical and technical (5 marks)
-- **THEi Identification**: Correctly identifying that THEi focuses on vocationally-oriented **Bachelor’s Degree** programmes (5 marks)
-**General Rubric Application:**
-- **9-10 marks**: Complete, accurate, uses correct terminology, and well-explained.
-- **6-8 marks**: Mostly correct but misses a specific detail or explanation is slightly vague.
-- **3-5 marks**: Basic understanding but misses core point or only answers half the question.
-- **0-2 marks**: Incorrect, irrelevant, or blank.
+          <t>- **IVE**: Primarily focuses on **Higher Diploma (HD)** programmes which are practical and technical in nature (5 marks)
+- **THEi**: Focuses on vocationally-oriented **Bachelor’s Degree** programmes that combine practical application with higher-level theory (5 marks)
+**General Grading Principles:**
+- **9-10 marks**: Complete, accurate, correct terminology.
+- **6-8 marks**: Mostly correct, misses detail.
+- **3-5 marks**: Basic understanding only.
+- **0-2 marks**: Incorrect or irrelevant.
 ---
 **General Grading Guide:**
 - **9-10 marks**: The answer is complete, accurate, uses correct terminology, and is well-explained.
@@ -531,19 +531,19 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Educational Philosophy. VTC emphasizes the "Think and Do" approach. Explain what this phrase means in the context of a student's learning experience.</t>
+          <t>VTC emphasizes the " Think and Do" approach. Explain what this phrase means in the context of a student's learning experience.</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>- **"Think" Component**: Explaining the application of brainpower, theory, or academic knowledge (3 marks)
-- **"Do" Component**: Explaining the application of practical work, hands-on technical skills, or execution (3 marks)
-- **Synthesis**: Explaining the ability to solve problems by combining both head and hands (4 marks)
-**General Rubric Application:**
-- **9-10 marks**: Complete, accurate, uses correct terminology, and well-explained.
-- **6-8 marks**: Mostly correct but misses a specific detail or explanation is slightly vague.
-- **3-5 marks**: Basic understanding but misses core point or only answers half the question.
-- **0-2 marks**: Incorrect, irrelevant, or blank.
+          <t>- **Think**: Theory/Academic knowledge/Brainpower (3 marks)
+- **Do**: Practical skills/Hands-on/Technical execution (3 marks)
+- **Synthesis**: Ability to solve problems by combining both head and hands (4 marks)
+**General Grading Principles:**
+- **9-10 marks**: Complete, accurate, correct terminology.
+- **6-8 marks**: Mostly correct, misses detail.
+- **3-5 marks**: Basic understanding only.
+- **0-2 marks**: Incorrect or irrelevant.
 ---
 **General Grading Guide:**
 - **9-10 marks**: The answer is complete, accurate, uses correct terminology, and is well-explained.
@@ -564,18 +564,18 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Study Pathways. If a Secondary 6 student does not achieve the minimum entrance requirements for a Bachelor's Degree or a Higher Diploma, what is the VTC study pathway available to them to eventually reach a Higher Diploma level? (Name the specific foundation programme).</t>
+          <t>If a Secondary 6 student does not achieve the minimum entrance requirements for a Bachelor's Degree or a Higher Diploma, what is the VTC study pathway available to them to eventually reach a Higher Diploma level? (Name the specific foundation programme).</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>- **Programme Name**: Correctly naming the **Diploma of Foundation Studies (DFS)** or **Diploma of Vocational Education (DVE)** (5 marks)
-- **Progression Path**: Explaining that successful completion allows progression to **Higher Diploma (HD)** programmes (5 marks)
-**General Rubric Application:**
-- **9-10 marks**: Complete, accurate, uses correct terminology, and well-explained.
-- **6-8 marks**: Mostly correct but misses a specific detail or explanation is slightly vague.
-- **3-5 marks**: Basic understanding but misses core point or only answers half the question.
-- **0-2 marks**: Incorrect, irrelevant, or blank.
+          <t>- Correctly naming the **Diploma of Foundation Studies (DFS)** or **Diploma of Vocational Education (DVE)** (5 marks)
+- Explanation of progression: Successful completion allows entry to **Higher Diploma (HD)** programmes (5 marks)
+**General Grading Principles:**
+- **9-10 marks**: Complete, accurate, correct terminology.
+- **6-8 marks**: Mostly correct, misses detail.
+- **3-5 marks**: Basic understanding only.
+- **0-2 marks**: Incorrect or irrelevant.
 ---
 **General Grading Guide:**
 - **9-10 marks**: The answer is complete, accurate, uses correct terminology, and is well-explained.
@@ -596,19 +596,19 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Industry Partnership. Why does the VTC collaborate closely with industry partners (companies and trade associations)? Give two examples of how this benefits students.</t>
+          <t>Why does the VTC collaborate closely with industry partners (companies and trade associations)? Give two examples of how this benefits students.</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>- **General Rationale**: Ensuring curriculum is up-to-date with market trends and industry needs (4 marks)
-- **Benefit Example 1**: Specific benefit such as **internships** or work-integrated learning (3 marks)
-- **Benefit Example 2**: Specific benefit such as **job placement support** or access to industry-standard equipment (3 marks)
-**General Rubric Application:**
-- **9-10 marks**: Complete, accurate, uses correct terminology, and well-explained.
-- **6-8 marks**: Mostly correct but misses a specific detail or explanation is slightly vague.
-- **3-5 marks**: Basic understanding but misses core point or only answers half the question.
-- **0-2 marks**: Incorrect, irrelevant, or blank.
+          <t>- **General Explanation**: Ensures curriculum is up-to-date with market trends and industry needs (4 marks)
+- **Benefit 1**: e.g., **Internship** or Work-integrated learning opportunities (3 marks)
+- **Benefit 2**: e.g., **Job placement support** or access to industry-standard equipment (3 marks)
+**General Grading Principles:**
+- **9-10 marks**: Complete, accurate, correct terminology.
+- **6-8 marks**: Mostly correct, misses detail.
+- **3-5 marks**: Basic understanding only.
+- **0-2 marks**: Incorrect or irrelevant.
 ---
 **General Grading Guide:**
 - **9-10 marks**: The answer is complete, accurate, uses correct terminology, and is well-explained.
@@ -712,7 +712,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2026-01-06 06:20:04</t>
+          <t>2026-01-07 02:18:41</t>
         </is>
       </c>
     </row>
@@ -784,7 +784,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>The Role of VTC. The VTC is the largest provider of VPET in Hong Kong. Briefly explain what VPET stands for and why it is important for Hong Kong’s workforce development.</t>
+          <t>The VTC is the largest provider of VPET in Hong Kong. Briefly explain what VPET stands for and why it is important for Hong Kong’s workforce development.</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -799,7 +799,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Member Institutions. Compare IVE (Hong Kong Institute of Vocational Education) and THEi (Technological and Higher Education Institute of Hong Kong). What is the main difference between the types of qualifications/programmes offered by these two institutions?</t>
+          <t>Compare IVE (Hong Kong Institute of Vocational Education) and THEi (Technological and Higher Education Institute of Hong Kong). What is the main difference between the types of qualifications/programmes offered by these two institutions?</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -814,7 +814,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Educational Philosophy. VTC emphasizes the "Think and Do" approach. Explain what this phrase means in the context of a student's learning experience.</t>
+          <t>VTC emphasizes the " Think and Do" approach. Explain what this phrase means in the context of a student's learning experience.</t>
         </is>
       </c>
       <c r="C4" t="n">
@@ -829,7 +829,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Study Pathways. If a Secondary 6 student does not achieve the minimum entrance requirements for a Bachelor's Degree or a Higher Diploma, what is the VTC study pathway available to them to eventually reach a Higher Diploma level? (Name the specific foundation programme).</t>
+          <t>If a Secondary 6 student does not achieve the minimum entrance requirements for a Bachelor's Degree or a Higher Diploma, what is the VTC study pathway available to them to eventually reach a Higher Diploma level? (Name the specific foundation programme).</t>
         </is>
       </c>
       <c r="C5" t="n">
@@ -844,7 +844,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Industry Partnership. Why does the VTC collaborate closely with industry partners (companies and trade associations)? Give two examples of how this benefits students.</t>
+          <t>Why does the VTC collaborate closely with industry partners (companies and trade associations)? Give two examples of how this benefits students.</t>
         </is>
       </c>
       <c r="C6" t="n">

</xml_diff>

<commit_message>
Move caching logic from notebook to agents.
</commit_message>
<xml_diff>
--- a/sample/VTC Test Marking Scheme.xlsx
+++ b/sample/VTC Test Marking Scheme.xlsx
@@ -466,25 +466,24 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>The VTC is the largest provider of VPET in Hong Kong. Briefly explain what VPET stands for and why it is important for Hong Kong’s workforce development.</t>
+          <t>The VTC is the largest provider of **VPET** in Hong Kong. Briefly explain what **VPET** stands for and why it is important for Hong Kong’s workforce development.</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>- **Vocational and Professional Education and Training** (2 marks)
-- Focus on **practical skills** or **specialized trades** (4 marks)
-- Benefit to workforce: reducing skills gap, employment readiness (4 marks)
-**General Grading Principles:**
-- **9-10 marks**: Complete, accurate, correct terminology.
-- **6-8 marks**: Mostly correct, misses detail.
-- **3-5 marks**: Basic understanding only.
-- **0-2 marks**: Incorrect or irrelevant.
+          <t>**Model Answer:**
+VPET stands for **Vocational and Professional Education and Training**. It is important because it provides students with practical skills and specialized knowledge needed by industries, ensuring Hong Kong has a skilled labor force to support the economy.
+**Marking Breakdown:**
+- Correctly stating "Vocational and Professional Education and Training" **(2 marks)**
+- Explaining that it focuses on _practical skills_ or _specialized trades_ **(4 marks)**
+- Explaining the benefit to the workforce (reducing skills gap, employment readiness) **(4 marks)**
 ---
 **General Grading Guide:**
-- **9-10 marks**: The answer is complete, accurate, uses correct terminology, and is well-explained.
-- **6-8 marks**: The answer is mostly correct but misses a specific detail (e.g., forgets the full name of a diploma) or the explanation is slightly vague.
-- **3-5 marks**: The student shows basic understanding but misses the core point or only answers half the question.
-- **0-2 marks**: The answer is largely incorrect, irrelevant, or blank.</t>
+**General Grading Guide (for partial marks)**
+- **9-10 marks:** The answer is complete, accurate, uses correct terminology, and is well-explained.
+- **6-8 marks:** The answer is mostly correct but misses a specific detail (e.g., forgets the full name of a diploma) or the explanation is slightly vague.
+- **3-5 marks:** The student shows basic understanding but misses the core point or only answers half the question.
+- **0-2 marks:** The answer is largely incorrect, irrelevant, or blank.</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -499,24 +498,23 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Compare IVE (Hong Kong Institute of Vocational Education) and THEi (Technological and Higher Education Institute of Hong Kong). What is the main difference between the types of qualifications/programmes offered by these two institutions?</t>
+          <t>Compare **IVE (Hong Kong Institute of Vocational Education)** and **THEi (Technological and Higher Education Institute of Hong Kong)**. What is the main difference between the types of qualifications/programmes offered by these two institutions?</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>- **IVE**: Primarily focuses on **Higher Diploma (HD)** programmes which are practical and technical in nature (5 marks)
-- **THEi**: Focuses on vocationally-oriented **Bachelor’s Degree** programmes that combine practical application with higher-level theory (5 marks)
-**General Grading Principles:**
-- **9-10 marks**: Complete, accurate, correct terminology.
-- **6-8 marks**: Mostly correct, misses detail.
-- **3-5 marks**: Basic understanding only.
-- **0-2 marks**: Incorrect or irrelevant.
+          <t>**Model Answer:**
+**IVE** primarily focuses on **Higher Diploma (HD)** programmes which are practical and technical in nature. **THEi** focuses on vocationally-oriented **Bachelor’s Degree** programmes that combine practical application with higher-level theory.
+**Marking Breakdown:**
+- Correctly identifying that IVE offers Higher Diplomas/Technical training **(5 marks)**
+- Correctly identifying that THEi offers Bachelor's Degrees **(5 marks)**
 ---
 **General Grading Guide:**
-- **9-10 marks**: The answer is complete, accurate, uses correct terminology, and is well-explained.
-- **6-8 marks**: The answer is mostly correct but misses a specific detail (e.g., forgets the full name of a diploma) or the explanation is slightly vague.
-- **3-5 marks**: The student shows basic understanding but misses the core point or only answers half the question.
-- **0-2 marks**: The answer is largely incorrect, irrelevant, or blank.</t>
+**General Grading Guide (for partial marks)**
+- **9-10 marks:** The answer is complete, accurate, uses correct terminology, and is well-explained.
+- **6-8 marks:** The answer is mostly correct but misses a specific detail (e.g., forgets the full name of a diploma) or the explanation is slightly vague.
+- **3-5 marks:** The student shows basic understanding but misses the core point or only answers half the question.
+- **0-2 marks:** The answer is largely incorrect, irrelevant, or blank.</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -531,25 +529,24 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>VTC emphasizes the " Think and Do" approach. Explain what this phrase means in the context of a student's learning experience.</t>
+          <t>VTC emphasizes the **" Think and Do"** approach. Explain what this phrase means in the context of a student's learning experience.</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>- **Think**: Theory/Academic knowledge/Brainpower (3 marks)
-- **Do**: Practical skills/Hands-on/Technical execution (3 marks)
-- **Synthesis**: Ability to solve problems by combining both head and hands (4 marks)
-**General Grading Principles:**
-- **9-10 marks**: Complete, accurate, correct terminology.
-- **6-8 marks**: Mostly correct, misses detail.
-- **3-5 marks**: Basic understanding only.
-- **0-2 marks**: Incorrect or irrelevant.
+          <t>**Model Answer:**
+This approach cultivates the ability to apply brainpower (theory/thinking) to practical work (doing). It ensures students understand the theory behind their work while also possessing the hands-on technical skills to execute it.
+**Marking Breakdown:**
+- Explaining "Think" (Theory/Academic knowledge) **(3 marks)**
+- Explaining "Do" (Practical skills/Hands-on) **(3 marks)**
+- Explaining the synthesis: Being able to solve problems by combining both head and hands **(4 marks)**
 ---
 **General Grading Guide:**
-- **9-10 marks**: The answer is complete, accurate, uses correct terminology, and is well-explained.
-- **6-8 marks**: The answer is mostly correct but misses a specific detail (e.g., forgets the full name of a diploma) or the explanation is slightly vague.
-- **3-5 marks**: The student shows basic understanding but misses the core point or only answers half the question.
-- **0-2 marks**: The answer is largely incorrect, irrelevant, or blank.</t>
+**General Grading Guide (for partial marks)**
+- **9-10 marks:** The answer is complete, accurate, uses correct terminology, and is well-explained.
+- **6-8 marks:** The answer is mostly correct but misses a specific detail (e.g., forgets the full name of a diploma) or the explanation is slightly vague.
+- **3-5 marks:** The student shows basic understanding but misses the core point or only answers half the question.
+- **0-2 marks:** The answer is largely incorrect, irrelevant, or blank.</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -564,24 +561,23 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>If a Secondary 6 student does not achieve the minimum entrance requirements for a Bachelor's Degree or a Higher Diploma, what is the VTC study pathway available to them to eventually reach a Higher Diploma level? (Name the specific foundation programme).</t>
+          <t>If a Secondary 6 student does **not** achieve the minimum entrance requirements for a Bachelor's Degree or a Higher Diploma, what is the VTC study pathway available to them to eventually reach a Higher Diploma level? (Name the specific foundation programme).</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>- Correctly naming the **Diploma of Foundation Studies (DFS)** or **Diploma of Vocational Education (DVE)** (5 marks)
-- Explanation of progression: Successful completion allows entry to **Higher Diploma (HD)** programmes (5 marks)
-**General Grading Principles:**
-- **9-10 marks**: Complete, accurate, correct terminology.
-- **6-8 marks**: Mostly correct, misses detail.
-- **3-5 marks**: Basic understanding only.
-- **0-2 marks**: Incorrect or irrelevant.
+          <t>**Model Answer:**
+The student can enroll in the **Diploma of Foundation Studies (DFS)** (or Diploma of Vocational Education). Upon successful completion of this diploma, they are eligible to progress to VTC **Higher Diploma (HD)** programmes.
+**Marking Breakdown:**
+- Correctly naming the "Diploma of Foundation Studies" (DFS) or "Diploma of Vocational Education" (DVE) **(5 marks)**
+- Explanation of the progression (Completion of DFS guarantees/allows entry to Higher Diploma) **(5 marks)**
 ---
 **General Grading Guide:**
-- **9-10 marks**: The answer is complete, accurate, uses correct terminology, and is well-explained.
-- **6-8 marks**: The answer is mostly correct but misses a specific detail (e.g., forgets the full name of a diploma) or the explanation is slightly vague.
-- **3-5 marks**: The student shows basic understanding but misses the core point or only answers half the question.
-- **0-2 marks**: The answer is largely incorrect, irrelevant, or blank.</t>
+**General Grading Guide (for partial marks)**
+- **9-10 marks:** The answer is complete, accurate, uses correct terminology, and is well-explained.
+- **6-8 marks:** The answer is mostly correct but misses a specific detail (e.g., forgets the full name of a diploma) or the explanation is slightly vague.
+- **3-5 marks:** The student shows basic understanding but misses the core point or only answers half the question.
+- **0-2 marks:** The answer is largely incorrect, irrelevant, or blank.</t>
         </is>
       </c>
       <c r="D5" t="n">
@@ -596,25 +592,24 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Why does the VTC collaborate closely with industry partners (companies and trade associations)? Give two examples of how this benefits students.</t>
+          <t>Why does the VTC collaborate closely with industry partners (companies and trade associations)? Give **two** examples of how this benefits students.</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>- **General Explanation**: Ensures curriculum is up-to-date with market trends and industry needs (4 marks)
-- **Benefit 1**: e.g., **Internship** or Work-integrated learning opportunities (3 marks)
-- **Benefit 2**: e.g., **Job placement support** or access to industry-standard equipment (3 marks)
-**General Grading Principles:**
-- **9-10 marks**: Complete, accurate, correct terminology.
-- **6-8 marks**: Mostly correct, misses detail.
-- **3-5 marks**: Basic understanding only.
-- **0-2 marks**: Incorrect or irrelevant.
+          <t>**Model Answer:**
+Collaboration ensures the curriculum is up-to-date with market trends. Benefits include: (1) Internship/Work-integrated learning opportunities, (2) Job placement support, (3) Access to industry-standard equipment/facilities.
+**Marking Breakdown:**
+- General explanation (Curriculum relevance/Industry needs) **(4 marks)**
+- First specific benefit (e.g., Internships) **(3 marks)**
+- Second specific benefit (e.g., Job prospects or Equipment) **(3 marks)**
 ---
 **General Grading Guide:**
-- **9-10 marks**: The answer is complete, accurate, uses correct terminology, and is well-explained.
-- **6-8 marks**: The answer is mostly correct but misses a specific detail (e.g., forgets the full name of a diploma) or the explanation is slightly vague.
-- **3-5 marks**: The student shows basic understanding but misses the core point or only answers half the question.
-- **0-2 marks**: The answer is largely incorrect, irrelevant, or blank.</t>
+**General Grading Guide (for partial marks)**
+- **9-10 marks:** The answer is complete, accurate, uses correct terminology, and is well-explained.
+- **6-8 marks:** The answer is mostly correct but misses a specific detail (e.g., forgets the full name of a diploma) or the explanation is slightly vague.
+- **3-5 marks:** The student shows basic understanding but misses the core point or only answers half the question.
+- **0-2 marks:** The answer is largely incorrect, irrelevant, or blank.</t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -712,7 +707,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2026-01-07 02:18:41</t>
+          <t>2026-01-07 03:42:00</t>
         </is>
       </c>
     </row>
@@ -784,7 +779,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>The VTC is the largest provider of VPET in Hong Kong. Briefly explain what VPET stands for and why it is important for Hong Kong’s workforce development.</t>
+          <t>The VTC is the largest provider of **VPET** in Hong Kong. Briefly explain what **VPET** stands for and why it is important for Hong Kong’s workforce development.</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -799,7 +794,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Compare IVE (Hong Kong Institute of Vocational Education) and THEi (Technological and Higher Education Institute of Hong Kong). What is the main difference between the types of qualifications/programmes offered by these two institutions?</t>
+          <t>Compare **IVE (Hong Kong Institute of Vocational Education)** and **THEi (Technological and Higher Education Institute of Hong Kong)**. What is the main difference between the types of qualifications/programmes offered by these two institutions?</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -814,7 +809,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>VTC emphasizes the " Think and Do" approach. Explain what this phrase means in the context of a student's learning experience.</t>
+          <t>VTC emphasizes the **" Think and Do"** approach. Explain what this phrase means in the context of a student's learning experience.</t>
         </is>
       </c>
       <c r="C4" t="n">
@@ -829,7 +824,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>If a Secondary 6 student does not achieve the minimum entrance requirements for a Bachelor's Degree or a Higher Diploma, what is the VTC study pathway available to them to eventually reach a Higher Diploma level? (Name the specific foundation programme).</t>
+          <t>If a Secondary 6 student does **not** achieve the minimum entrance requirements for a Bachelor's Degree or a Higher Diploma, what is the VTC study pathway available to them to eventually reach a Higher Diploma level? (Name the specific foundation programme).</t>
         </is>
       </c>
       <c r="C5" t="n">
@@ -844,7 +839,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Why does the VTC collaborate closely with industry partners (companies and trade associations)? Give two examples of how this benefits students.</t>
+          <t>Why does the VTC collaborate closely with industry partners (companies and trade associations)? Give **two** examples of how this benefits students.</t>
         </is>
       </c>
       <c r="C6" t="n">

</xml_diff>

<commit_message>
add marking scheme Verification
</commit_message>
<xml_diff>
--- a/sample/VTC Test Marking Scheme.xlsx
+++ b/sample/VTC Test Marking Scheme.xlsx
@@ -11,6 +11,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Summary" sheetId="2" state="visible" r:id="rId2"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Question Overview" sheetId="3" state="visible" r:id="rId3"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Validation" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Content Verification" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -627,7 +628,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -702,34 +703,46 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Generated On</t>
+          <t>Verification Feedback</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2026-01-07 03:42:00</t>
+          <t>Overall Evaluation Summary: The marking scheme is factually accurate and aligns with the official terminology, institutional roles, and educational pathways defined by the VTC. The marking breakdowns are logical and prioritize the most critical information. Final Recommendations: 1. Terminology Consistency: Ensure that 'Vocational and Professional Education and Training' is always written in full for the 2-mark component of Q1 to avoid ambiguity. 2. Partial Marks: The 'General Grading Guide' is helpful, but for Q2 and Q4, ensure examiners know that naming the specific qualification (Higher Diploma vs. Degree or DFS) is the 'hurdle' requirement for moving above the 5-mark threshold. 3. Wording Improvement: In Q4, the phrase 'guarantees entry' should be used cautiously; 'eligibility to apply' or 'articulation pathway' is more technically accurate as some HD programs have specific interviews or subject requirements. Citations: vtc.edu.hk, iabhongkong.com, legco.gov.hk.</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Input File</t>
+          <t>Generated On</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>VTC Test Marking Scheme.docx</t>
+          <t>2026-01-07 13:54:45</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
+          <t>Input File</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>VTC Test Marking Scheme.docx</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
           <t>Output File</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="B10" t="inlineStr">
         <is>
           <t>VTC Test Marking Scheme.xlsx</t>
         </is>
@@ -940,4 +953,145 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>question_number</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>is_correct</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>feedback</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>suggestion</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Q1</t>
+        </is>
+      </c>
+      <c r="B2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Fact Check: Correct. VPET stands for Vocational and Professional Education and Training. The VTC is officially recognized as the largest provider of VPET in Hong Kong. Verification Detail: Official VTC corporate information and annual reports confirm this acronym and the council's status as the primary statutory body for vocational training.</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>The answer is solid. To make the 'Importance' section even more robust, you could mention that VPET is a 'valued choice' alongside traditional academic paths, which is a key part of the Hong Kong government's recent branding of the sector.</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Q2</t>
+        </is>
+      </c>
+      <c r="B3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Fact Check: Correct. IVE (Hong Kong Institute of Vocational Education) is the primary provider of Higher Diplomas (HD) and Certificates. THEi (Technological and Higher Education Institute of Hong Kong) was specifically established to offer vocationally-oriented Bachelor’s Degrees. Verification Detail: While THEi does offer a small number of Higher Diplomas, its defining characteristic in the VTC ecosystem is providing the degree-level 'top' of the progression ladder.</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>The marking breakdown is fair. You might add a note for examiners that mentioning 'Applied Degrees' is also a highly accurate description for THEi.</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Q3</t>
+        </is>
+      </c>
+      <c r="B4" t="b">
+        <v>1</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Fact Check: Correct. 'Think and Do' is the official motto and pedagogical approach of the VTC. Verification Detail: VTC branding materials emphasize this approach to distinguish their training from purely theoretical academic studies. It specifically refers to the integration of 'Head' (knowledge) and 'Hands' (skills).</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>The marking breakdown is excellent. Ensure students understand that 'Think' refers to professional knowledge/theory, not just general thinking.</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Q4</t>
+        </is>
+      </c>
+      <c r="B5" t="b">
+        <v>1</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Fact Check: Correct. The Diploma of Foundation Studies (DFS) is the standard one-year program for S6 leavers to bridge into a Higher Diploma. The Diploma of Vocational Education (DVE) is also a valid pathway (offered by Youth College). Verification Detail: VTC admission guides list DFS as the primary 'Level 3' qualification on the Qualifications Framework (QF) that grants eligibility for HD programs.</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>You may want to mention the Diploma of Applied Education (DAE) as an alternative, though DFS/DVE are the specific VTC-branded programs. The current answer is the most relevant for a VTC-specific context.</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Q5</t>
+        </is>
+      </c>
+      <c r="B6" t="b">
+        <v>1</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Fact Check: Correct. VTC operates 25 Training Boards that represent various industries to ensure curriculum relevance. Verification Detail: Key benefits include Work-Integrated Learning (WIL), which is the formal term VTC uses for internships, and the use of industry-donated facilities (e.g., the Boeing-standard engine in their engineering labs).</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>The examples provided (Internships, Job Placement, Equipment) are the most common and correct answers. Using the term 'Work-Integrated Learning (WIL)' could be a 'bonus' keyword for a 10-mark answer.</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update Word doc structure and README.
</commit_message>
<xml_diff>
--- a/sample/VTC Test Marking Scheme.xlsx
+++ b/sample/VTC Test Marking Scheme.xlsx
@@ -708,7 +708,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Overall Evaluation Summary: The marking scheme is factually accurate and aligns with the official terminology, institutional roles, and educational pathways defined by the VTC. The marking breakdowns are logical and prioritize the most critical information. Final Recommendations: 1. Terminology Consistency: Ensure that 'Vocational and Professional Education and Training' is always written in full for the 2-mark component of Q1 to avoid ambiguity. 2. Partial Marks: The 'General Grading Guide' is helpful, but for Q2 and Q4, ensure examiners know that naming the specific qualification (Higher Diploma vs. Degree or DFS) is the 'hurdle' requirement for moving above the 5-mark threshold. 3. Wording Improvement: In Q4, the phrase 'guarantees entry' should be used cautiously; 'eligibility to apply' or 'articulation pathway' is more technically accurate as some HD programs have specific interviews or subject requirements. Citations: vtc.edu.hk, iabhongkong.com, legco.gov.hk.</t>
+          <t>The marking scheme is highly accurate and ready for use. The terminology matches current Hong Kong educational policy (VPET) and VTC’s institutional structure. No factual errors were found. This evaluation confirms that the marking scheme is factually accurate and aligns with the official standards and terminology of the Vocational Training Council (VTC) in Hong Kong. [vtc.edu.hk](https://vertexaisearch.cloud.google.com/grounding-api-redirect/AUZIYQGfYjWT3BilK0Z-osBdBJkrXPQjTZDsS96PhghiYYnUHdoFpqFUpVSQHZDE4dIKCXYhvEE8x1Z4-BwC-kdHBBBLMTaY8h9bLVoJhUOxj-2i2_Jt848kCldR_bb5ZQ3CyZuT4EUrO9Yj)</t>
         </is>
       </c>
     </row>
@@ -720,7 +720,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2026-01-07 13:54:45</t>
+          <t>2026-01-07 14:20:19</t>
         </is>
       </c>
     </row>
@@ -1002,12 +1002,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Fact Check: Correct. VPET stands for Vocational and Professional Education and Training. The VTC is officially recognized as the largest provider of VPET in Hong Kong. Verification Detail: Official VTC corporate information and annual reports confirm this acronym and the council's status as the primary statutory body for vocational training.</t>
+          <t>Terminology is 100% correct. VTC is officially recognized as the largest VPET provider in HK. According to the Hong Kong Education Bureau (EDB) and VTC corporate documents, VPET stands for Vocational and Professional Education and Training. VTC is indeed the largest provider, serving over 200,000 students annually. [vtc.edu.hk](https://vertexaisearch.cloud.google.com/grounding-api-redirect/AUZIYQGXnV_z3VfqDjGu28vBBuPopdDzvAy0H5JnyvN-0fZvBU_rcHRuERR8w7TzXA5U3LzaFmmxiUo_5iKb8ch-sNZok_mgIJlO9QFl0r9JixDHfRw5-TS_gF_ma1Y=)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>The answer is solid. To make the 'Importance' section even more robust, you could mention that VPET is a 'valued choice' alongside traditional academic paths, which is a key part of the Hong Kong government's recent branding of the sector.</t>
+          <t>The marking scheme is excellent. To make it even more robust, you could mention that VPET is recognized under the Hong Kong Qualifications Framework (HKQF) to emphasize its formal status.</t>
         </is>
       </c>
     </row>
@@ -1022,12 +1022,12 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Fact Check: Correct. IVE (Hong Kong Institute of Vocational Education) is the primary provider of Higher Diplomas (HD) and Certificates. THEi (Technological and Higher Education Institute of Hong Kong) was specifically established to offer vocationally-oriented Bachelor’s Degrees. Verification Detail: While THEi does offer a small number of Higher Diplomas, its defining characteristic in the VTC ecosystem is providing the degree-level 'top' of the progression ladder.</t>
+          <t>Correctly distinguishes between the sub-degree (IVE) and degree (THEi) levels. IVE (Hong Kong Institute of Vocational Education) is the primary member institution for Higher Diplomas. THEi (Technological and Higher Education Institute of Hong Kong) was specifically established to offer vocationally-oriented Bachelor’s Degrees. [apqn.org](https://vertexaisearch.cloud.google.com/grounding-api-redirect/AUZIYQHfJJY7QCN6DCC9qBFoBZZW_kLBax2iyr-W9BtD79JuasnZbUtE6JbYEUPxCxFoU0mVdszotrSNl4En9a-dNzkWcOQhSfLz2pgFUX6CfXoerxLfsR2t_yfQAx5v3xYLbAyqVgd2Ss3xHUNuOSemW_Gl73zrWrsHSqo=)</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>The marking breakdown is fair. You might add a note for examiners that mentioning 'Applied Degrees' is also a highly accurate description for THEi.</t>
+          <t>The answer is correct. You might add that THEi degrees are often "Applied Degrees," which is a specific term currently promoted by the EDB.</t>
         </is>
       </c>
     </row>
@@ -1042,12 +1042,12 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Fact Check: Correct. 'Think and Do' is the official motto and pedagogical approach of the VTC. Verification Detail: VTC branding materials emphasize this approach to distinguish their training from purely theoretical academic studies. It specifically refers to the integration of 'Head' (knowledge) and 'Hands' (skills).</t>
+          <t>This is the official VTC motto. The explanation of theory vs. practice is accurate. VTC’s official branding frequently uses the phrase "Think and Do" (sometimes paired with "Hands-on, Minds-on"). It refers to the integration of theoretical knowledge with practical application. [vtc.edu.hk](https://vertexaisearch.cloud.google.com/grounding-api-redirect/AUZIYQHDbintfm2E7gNTfbWuVqyf9FvW7zrwNcMEOKd3Uo9xfb_TXpbT5trnUT3u5ZWbshmBj0eCp5Ig0B-4BUSk0JcyCpjzS3nP6Yj-C1bK2h0HYJJmKhoGD0v4WxTxT_2NaMn4OT3HbrpnRdl-5KlKPLv_ElwCA==)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>The marking breakdown is excellent. Ensure students understand that 'Think' refers to professional knowledge/theory, not just general thinking.</t>
+          <t>The marking breakdown is well-balanced. Ensure students understand that "Think" isn't just "remembering facts" but "problem-solving and analytical thinking."</t>
         </is>
       </c>
     </row>
@@ -1062,12 +1062,12 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Fact Check: Correct. The Diploma of Foundation Studies (DFS) is the standard one-year program for S6 leavers to bridge into a Higher Diploma. The Diploma of Vocational Education (DVE) is also a valid pathway (offered by Youth College). Verification Detail: VTC admission guides list DFS as the primary 'Level 3' qualification on the Qualifications Framework (QF) that grants eligibility for HD programs.</t>
+          <t>DFS and DVE are the standard "bridge" programmes for S6 students. For S6 students who do not meet the "3322+2" (Degree) or "22222" (HD) DSE requirements, the Diploma of Foundation Studies (DFS) is the standard one-year progression route. The Diploma of Vocational Education (DVE) is also a valid answer, typically offered by Youth College. [vtc.edu.hk](https://vertexaisearch.cloud.google.com/grounding-api-redirect/AUZIYQFk0SBJGwIzx2bq4cHmucdpXKcFbf8_K2l1Uicysm9GGnfQmybL0cEF8kGz5lGHU8x1DeP1g0ZCMPsR_ARpYI8irjnn4Ycl11KBmNbimHQu3omhmH6Ekq_klGPT17wI714YDkfP_JODmtafU0GWRlPtZO4Jfk2DNRWJiiUltvp-pV7HIg==)</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>You may want to mention the Diploma of Applied Education (DAE) as an alternative, though DFS/DVE are the specific VTC-branded programs. The current answer is the most relevant for a VTC-specific context.</t>
+          <t>The answer is accurate. Note that successful completion of DFS is considered equivalent to Level 2 in five DSE subjects (including English and Chinese) for civil service applications, which is a major "importance" factor you could include.</t>
         </is>
       </c>
     </row>
@@ -1082,12 +1082,12 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Fact Check: Correct. VTC operates 25 Training Boards that represent various industries to ensure curriculum relevance. Verification Detail: Key benefits include Work-Integrated Learning (WIL), which is the formal term VTC uses for internships, and the use of industry-donated facilities (e.g., the Boeing-standard engine in their engineering labs).</t>
+          <t>Benefits listed (internships, equipment) are core pillars of VTC’s "Work-Integrated Learning." VTC operates under a "tripartite" model involving the government, industry, and the council. Work-Integrated Learning (WIL) and the VTC Earn &amp; Learn Scheme are real-world examples of this collaboration. [vtc.edu.hk](https://vertexaisearch.cloud.google.com/grounding-api-redirect/AUZIYQHwIxQUfSgNHoK6cwuQKfqGy010xqQsQ0Xpits1ZLg3iuvuTwFIxoe0JCSkhIaDZYw3kuDzP5t7rLPalvtMDy5FtsLTy8JT3IHuhjvK707d5tKiAtjeJArzHq2QqSU58pHznLcPz0g3mEdH2pHlwQbJ7IJM0AoN7RyyCKR0rt3K0A1kzueNR4A6C_lJakU=)</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>The examples provided (Internships, Job Placement, Equipment) are the most common and correct answers. Using the term 'Work-Integrated Learning (WIL)' could be a 'bonus' keyword for a 10-mark answer.</t>
+          <t>The examples provided (internships, equipment) are perfect. You could also suggest "Industry-endorsed curriculum" or "Professional recognition/certification" as alternative valid examples.</t>
         </is>
       </c>
     </row>

</xml_diff>